<commit_message>
Signed-off-by: STUDENT John Power <John.Power2@students.ittralee.ie>
</commit_message>
<xml_diff>
--- a/Assignment 1.xlsx
+++ b/Assignment 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20378"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00136836\Desktop\ComputerGraphics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACFA5B5B-1DEE-48CD-A57D-E9A7624182DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7415FC73-28FC-4493-BB5C-8D0E70A06938}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -461,34 +461,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -497,26 +503,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -862,7 +862,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -876,25 +876,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="K2" s="41" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="K2" s="28" t="s">
         <v>36</v>
       </c>
     </row>
@@ -912,7 +912,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K5" s="43" t="s">
+      <c r="K5" s="30" t="s">
         <v>37</v>
       </c>
     </row>
@@ -923,7 +923,7 @@
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="27">
         <f>MOD(C4,100)-50</f>
         <v>6</v>
       </c>
@@ -935,15 +935,15 @@
       <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="42">
+      <c r="C7" s="29">
         <f>INT((C4/10000))-5</f>
         <v>7</v>
       </c>
-      <c r="D7" s="42">
+      <c r="D7" s="29">
         <f>MOD(INT((C4/100)),10)-5</f>
         <v>-1</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="29">
         <f>MOD(INT((C4/100)),10)-5</f>
         <v>-1</v>
       </c>
@@ -955,19 +955,19 @@
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="31">
         <f>INT((C4/10000))-5</f>
         <v>7</v>
       </c>
-      <c r="D8" s="44">
+      <c r="D8" s="31">
         <f>MOD(INT((C4/1000)),10)-4</f>
         <v>-1</v>
       </c>
-      <c r="E8" s="44">
+      <c r="E8" s="31">
         <f>MOD(INT((C4/100)),10)-5</f>
         <v>-1</v>
       </c>
-      <c r="K8" s="45" t="s">
+      <c r="K8" s="32" t="s">
         <v>38</v>
       </c>
       <c r="L8" t="s">
@@ -981,15 +981,15 @@
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="40">
+      <c r="C9" s="27">
         <f>MOD(C4,10)-5</f>
         <v>1</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="27">
         <f>MOD(INT((C4/10)),10)-5</f>
         <v>0</v>
       </c>
-      <c r="E9" s="40">
+      <c r="E9" s="27">
         <f>MOD(INT((C4/100)),10)-4</f>
         <v>0</v>
       </c>
@@ -1001,15 +1001,15 @@
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="40">
+      <c r="C11" s="27">
         <f>2+C7</f>
         <v>9</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="27">
         <f>3+D7</f>
         <v>2</v>
       </c>
-      <c r="E11" s="40">
+      <c r="E11" s="27">
         <f>E7+50</f>
         <v>49</v>
       </c>
@@ -1019,15 +1019,15 @@
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="42">
+      <c r="C12" s="29">
         <f>D7</f>
         <v>-1</v>
       </c>
-      <c r="D12" s="42">
+      <c r="D12" s="29">
         <f>C8</f>
         <v>7</v>
       </c>
-      <c r="E12" s="42">
+      <c r="E12" s="29">
         <f>E8</f>
         <v>-1</v>
       </c>
@@ -1037,15 +1037,15 @@
       <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="42">
+      <c r="C13" s="29">
         <f>E9</f>
         <v>0</v>
       </c>
-      <c r="D13" s="42">
+      <c r="D13" s="29">
         <f>D7</f>
         <v>-1</v>
       </c>
-      <c r="E13" s="42">
+      <c r="E13" s="29">
         <f>C7</f>
         <v>7</v>
       </c>
@@ -1076,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1101,10 +1101,10 @@
     </row>
     <row r="2" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="5"/>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="30"/>
+      <c r="E2" s="38"/>
       <c r="F2" s="8"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1115,8 +1115,8 @@
     </row>
     <row r="3" spans="3:13" ht="111" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="5"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="32"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
       <c r="F3" s="6"/>
       <c r="G3" s="11"/>
       <c r="H3" s="7"/>
@@ -1136,10 +1136,10 @@
     </row>
     <row r="5" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="5"/>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="38"/>
       <c r="F5" s="8"/>
       <c r="H5" s="15"/>
       <c r="I5" s="12"/>
@@ -1148,8 +1148,8 @@
     </row>
     <row r="6" spans="3:13" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="5"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="32"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="36"/>
       <c r="F6" s="16"/>
       <c r="G6" s="12"/>
       <c r="H6" s="15"/>
@@ -1169,10 +1169,10 @@
     </row>
     <row r="8" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="5"/>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="30"/>
+      <c r="E8" s="38"/>
       <c r="F8" s="17"/>
       <c r="G8" s="12"/>
       <c r="H8" s="15"/>
@@ -1182,8 +1182,8 @@
     </row>
     <row r="9" spans="3:13" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="5"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="32"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="36"/>
       <c r="F9" s="17"/>
       <c r="G9" s="12"/>
       <c r="H9" s="15"/>
@@ -1203,28 +1203,28 @@
     </row>
     <row r="11" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="5"/>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="30"/>
+      <c r="E11" s="38"/>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="37" t="s">
+      <c r="H11" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="38"/>
+      <c r="I11" s="40"/>
       <c r="J11" s="8"/>
       <c r="L11" s="15"/>
       <c r="M11" s="12"/>
     </row>
     <row r="12" spans="3:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="5"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="39"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="43"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="39"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="43"/>
       <c r="J12" s="16"/>
       <c r="K12" s="12"/>
       <c r="L12" s="15"/>
@@ -1244,10 +1244,10 @@
     </row>
     <row r="14" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="5"/>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="30"/>
+      <c r="E14" s="38"/>
       <c r="F14" s="17"/>
       <c r="G14" s="12"/>
       <c r="H14" s="15"/>
@@ -1259,8 +1259,8 @@
     </row>
     <row r="15" spans="3:13" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="5"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="32"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="36"/>
       <c r="F15" s="17"/>
       <c r="G15" s="12"/>
       <c r="H15" s="15"/>
@@ -1284,10 +1284,10 @@
     </row>
     <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="5"/>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="30"/>
+      <c r="E17" s="38"/>
       <c r="F17" s="18"/>
       <c r="G17" s="12"/>
       <c r="H17" s="15"/>
@@ -1299,8 +1299,8 @@
     </row>
     <row r="18" spans="1:13" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="5"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="39"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="43"/>
       <c r="F18" s="20"/>
       <c r="H18" s="15"/>
       <c r="I18" s="12"/>
@@ -1321,18 +1321,18 @@
     </row>
     <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="5"/>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="30"/>
-      <c r="F20" s="34" t="s">
+      <c r="E20" s="38"/>
+      <c r="F20" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="36"/>
-      <c r="H20" s="37" t="s">
+      <c r="G20" s="42"/>
+      <c r="H20" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="38"/>
+      <c r="I20" s="40"/>
       <c r="J20" s="17"/>
       <c r="K20" s="12"/>
       <c r="L20" s="15"/>
@@ -1340,12 +1340,12 @@
     </row>
     <row r="21" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="5"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="39"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="43"/>
       <c r="J21" s="17"/>
       <c r="K21" s="12"/>
       <c r="L21" s="15"/>
@@ -1363,33 +1363,33 @@
     </row>
     <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="5"/>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="30"/>
+      <c r="E23" s="38"/>
       <c r="F23" s="9"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
       <c r="J23" s="10"/>
       <c r="K23" s="18"/>
-      <c r="L23" s="37" t="s">
+      <c r="L23" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="M23" s="38"/>
+      <c r="M23" s="40"/>
     </row>
     <row r="24" spans="1:13" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="5"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="39"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="43"/>
       <c r="F24" s="6"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="7"/>
       <c r="K24" s="23"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="39"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="43"/>
     </row>
     <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D25" s="13"/>
@@ -1402,10 +1402,10 @@
     <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="37" t="s">
+      <c r="D26" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="38"/>
+      <c r="E26" s="40"/>
       <c r="F26" s="12"/>
       <c r="J26" s="15"/>
       <c r="K26" s="12"/>
@@ -1416,8 +1416,8 @@
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="39"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="43"/>
       <c r="F27" s="12"/>
       <c r="J27" s="15"/>
       <c r="K27" s="12"/>
@@ -1435,15 +1435,15 @@
       <c r="M28" s="12"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="38"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="25"/>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="30"/>
+      <c r="E29" s="38"/>
       <c r="F29" s="9"/>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
@@ -1454,11 +1454,11 @@
       <c r="M29" s="12"/>
     </row>
     <row r="30" spans="1:13" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="33"/>
-      <c r="B30" s="39"/>
+      <c r="A30" s="35"/>
+      <c r="B30" s="43"/>
       <c r="C30" s="25"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="39"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="43"/>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
@@ -1476,44 +1476,44 @@
       <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="30"/>
+      <c r="B32" s="38"/>
       <c r="C32" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="30"/>
-      <c r="F32" s="34" t="s">
+      <c r="E32" s="38"/>
+      <c r="F32" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="29" t="s">
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="30"/>
+      <c r="M32" s="38"/>
     </row>
     <row r="33" spans="1:13" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="31"/>
-      <c r="B33" s="32"/>
+      <c r="A33" s="45"/>
+      <c r="B33" s="36"/>
       <c r="C33" s="17"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="35"/>
-      <c r="I33" s="35"/>
-      <c r="J33" s="35"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="32"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="42"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="36"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="21"/>
@@ -1525,32 +1525,47 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C35" s="5"/>
-      <c r="D35" s="37" t="s">
+      <c r="D35" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="E35" s="38"/>
+      <c r="E35" s="40"/>
       <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C36" s="5"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="39"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="43"/>
       <c r="F36" s="12"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E38" s="26"/>
       <c r="F38" s="26"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="32"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:K33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F32:K32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="D26:E26"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="F21:G21"/>
@@ -1565,27 +1580,12 @@
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F32:K32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>